<commit_message>
Updated web jobs with latest code
</commit_message>
<xml_diff>
--- a/Manual Deployment Guide/Scripts/webjobs/UploadScriptToADLS/scriptData/configuration/Configurations.xlsx
+++ b/Manual Deployment Guide/Scripts/webjobs/UploadScriptToADLS/scriptData/configuration/Configurations.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\honglu\git\Team Ilan\Projects\InventoryOptimization\configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmpechyo\Team%20Ilan\Projects\InventoryOptimization\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12696"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryPolicyConfig" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>ActiveFlag</t>
   </si>
@@ -574,27 +574,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="56" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="64" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +635,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -670,7 +670,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -705,7 +705,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -746,7 +746,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -784,7 +784,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -825,7 +825,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -866,7 +866,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -904,7 +904,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>0</v>
       </c>
@@ -945,7 +945,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -953,6 +953,9 @@
         <v>60</v>
       </c>
       <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
         <v>60</v>
       </c>
     </row>
@@ -970,16 +973,16 @@
       <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -996,7 +999,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>63</v>
       </c>
@@ -1112,14 +1115,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1141,7 +1144,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1166,9 +1169,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>

</xml_diff>